<commit_message>
Initial commit: Add existing project files
</commit_message>
<xml_diff>
--- a/BuyersAndSupplier.xlsx
+++ b/BuyersAndSupplier.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16935" windowHeight="5175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14760" windowHeight="3765"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
@@ -20,9 +20,6 @@
     <t>juli@poonamcoatings.com</t>
   </si>
   <si>
-    <t>Juli Co.</t>
-  </si>
-  <si>
     <t>juli@gmail.com</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>22AAAAA4000A3Z5</t>
   </si>
   <si>
-    <t>TestA</t>
-  </si>
-  <si>
     <t>TestB</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>Rajan</t>
+  </si>
+  <si>
+    <t>TestAA</t>
+  </si>
+  <si>
+    <t>Juli Co. Ltd</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,79 +536,79 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1">
-        <v>9878787678</v>
+        <v>9873787678</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1">
         <v>87878787</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
         <v>7878786776</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="J2" s="1">
         <v>100000</v>
@@ -617,46 +617,46 @@
         <v>30</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1">
         <v>382481</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>9838787678</v>
+        <v>9858787678</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1">
         <v>84878787</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>7871786776</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1">
         <v>200000</v>
@@ -665,46 +665,46 @@
         <v>60</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N3" s="1">
         <v>390002</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>9878587678</v>
+        <v>9878287678</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1">
         <v>87868787</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1">
         <v>7878586776</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4" s="1">
         <v>40000</v>
@@ -713,46 +713,46 @@
         <v>50</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N4" s="1">
         <v>392001</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>9878782678</v>
+        <v>9878792678</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>87878487</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G5" s="1">
         <v>7878786776</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5" s="1">
         <v>500000</v>
@@ -761,16 +761,16 @@
         <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N5" s="1">
         <v>390002</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q5" s="1"/>
     </row>

</xml_diff>